<commit_message>
FSDS Lecture code till Python and sql Intro
</commit_message>
<xml_diff>
--- a/Reference/FSDS_Schedule.xlsx
+++ b/Reference/FSDS_Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6800"/>
+    <workbookView windowWidth="18350" windowHeight="6080"/>
   </bookViews>
   <sheets>
     <sheet name="Lecture Plan" sheetId="1" r:id="rId1"/>
@@ -2164,8 +2164,8 @@
   <sheetPr/>
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -2286,36 +2286,36 @@
       <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" ht="40" customHeight="1" spans="1:7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>